<commit_message>
Dijital 19 2OK BCD3X, Dijital 19 BCD3X Paralel Vidalı ve Dijital 19 BCD3X Paralel Kablolu uzantıları eklendi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="91">
   <si>
     <t>Sıra</t>
   </si>
@@ -170,15 +170,9 @@
     <t>DP-EKA-DT-000-LIP-S2B1-01</t>
   </si>
   <si>
-    <t>DP-GLX-3X-000-LOP-P2B1-01</t>
-  </si>
-  <si>
     <t>3x Dot</t>
   </si>
   <si>
-    <t>DP-GLX-3X-000-LOP-P1B1-01</t>
-  </si>
-  <si>
     <t>DP-PNT-3X-000-LOP-P3B1-01</t>
   </si>
   <si>
@@ -288,13 +282,28 @@
   </si>
   <si>
     <t>EKA</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-DT-2OK-LIP-S2B1-01.git</t>
+  </si>
+  <si>
+    <t>DP-D19-3X-000-LOP-P2B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-3X-000-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-000-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-000-LOP-P2B1-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -324,6 +333,14 @@
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,10 +375,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -374,8 +392,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -656,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -672,7 +692,7 @@
     <col min="8" max="8" width="16.33203125" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="40.77734375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="49.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
@@ -740,7 +760,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K2" s="7"/>
     </row>
@@ -773,7 +793,7 @@
         <v>18</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K3" s="7"/>
     </row>
@@ -806,7 +826,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K4" s="7"/>
     </row>
@@ -839,7 +859,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K5" s="7"/>
     </row>
@@ -872,7 +892,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K6" s="7"/>
     </row>
@@ -905,7 +925,7 @@
         <v>18</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K7" s="7"/>
     </row>
@@ -938,7 +958,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K8" s="7"/>
     </row>
@@ -971,7 +991,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K9" s="7"/>
     </row>
@@ -1004,7 +1024,7 @@
         <v>18</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K10" s="7"/>
     </row>
@@ -1037,7 +1057,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K11" s="7"/>
     </row>
@@ -1070,7 +1090,7 @@
         <v>24</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K12" s="7"/>
     </row>
@@ -1103,7 +1123,7 @@
         <v>24</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K13" s="7"/>
     </row>
@@ -1136,7 +1156,7 @@
         <v>24</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K14" s="7"/>
     </row>
@@ -1169,7 +1189,7 @@
         <v>24</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K15" s="7"/>
     </row>
@@ -1202,7 +1222,7 @@
         <v>24</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K16" s="7"/>
     </row>
@@ -1214,7 +1234,7 @@
         <v>45</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>46</v>
@@ -1235,7 +1255,7 @@
         <v>24</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K17" s="7"/>
     </row>
@@ -1247,7 +1267,7 @@
         <v>47</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>46</v>
@@ -1268,7 +1288,7 @@
         <v>24</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K18" s="7"/>
     </row>
@@ -1277,14 +1297,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="E19" s="6" t="s">
         <v>14</v>
       </c>
@@ -1301,22 +1321,24 @@
         <v>24</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>14</v>
@@ -1334,22 +1356,24 @@
         <v>24</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K20" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>14</v>
@@ -1367,7 +1391,7 @@
         <v>24</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K21" s="7"/>
     </row>
@@ -1376,16 +1400,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>39</v>
@@ -1400,25 +1424,27 @@
         <v>24</v>
       </c>
       <c r="J22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>15</v>
@@ -1433,7 +1459,7 @@
         <v>24</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K23" s="7"/>
     </row>
@@ -1442,16 +1468,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>39</v>
@@ -1466,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K24" s="7"/>
     </row>
@@ -1475,13 +1501,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>37</v>
@@ -1499,7 +1525,7 @@
         <v>24</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K25" s="7"/>
     </row>
@@ -1508,13 +1534,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>14</v>
@@ -1532,7 +1558,7 @@
         <v>24</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K26" s="7"/>
     </row>
@@ -1541,13 +1567,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>37</v>
@@ -1565,7 +1591,7 @@
         <v>24</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K27" s="7"/>
     </row>
@@ -1574,22 +1600,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>43</v>
@@ -1598,7 +1624,7 @@
         <v>24</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K28" s="7"/>
     </row>
@@ -1607,13 +1633,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>14</v>
@@ -1631,7 +1657,7 @@
         <v>24</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K29" s="7"/>
     </row>
@@ -1640,19 +1666,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>16</v>
@@ -1664,7 +1690,7 @@
         <v>24</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K30" s="7"/>
     </row>
@@ -1673,13 +1699,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>37</v>
@@ -1697,7 +1723,7 @@
         <v>24</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K31" s="7"/>
     </row>
@@ -1706,19 +1732,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>22</v>
@@ -1730,7 +1756,7 @@
         <v>24</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K32" s="7"/>
     </row>
@@ -1739,20 +1765,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="G33" s="6" t="s">
         <v>16</v>
       </c>
@@ -1763,7 +1789,7 @@
         <v>24</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K33" s="7"/>
     </row>
@@ -1772,19 +1798,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="E34" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>16</v>
@@ -1796,7 +1822,7 @@
         <v>18</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K34" s="7"/>
     </row>
@@ -1805,19 +1831,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>16</v>
@@ -1829,7 +1855,7 @@
         <v>18</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K35" s="7"/>
     </row>
@@ -1838,7 +1864,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>33</v>
@@ -1850,7 +1876,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>16</v>
@@ -1862,7 +1888,7 @@
         <v>24</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K36" s="7"/>
     </row>
@@ -1871,7 +1897,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>33</v>
@@ -1883,7 +1909,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>16</v>
@@ -1895,7 +1921,7 @@
         <v>24</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K37" s="7"/>
     </row>
@@ -1904,7 +1930,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>33</v>
@@ -1916,7 +1942,7 @@
         <v>27</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>16</v>
@@ -1928,7 +1954,7 @@
         <v>24</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K38" s="7"/>
     </row>
@@ -1937,19 +1963,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>16</v>
@@ -1961,7 +1987,7 @@
         <v>24</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K39" s="7"/>
     </row>
@@ -1970,19 +1996,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>16</v>
@@ -1994,7 +2020,7 @@
         <v>24</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K40" s="7"/>
     </row>
@@ -2003,19 +2029,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>22</v>
@@ -2027,7 +2053,7 @@
         <v>24</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K41" s="7"/>
     </row>
@@ -2036,19 +2062,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>16</v>
@@ -2060,7 +2086,7 @@
         <v>24</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K42" s="7"/>
     </row>
@@ -2069,22 +2095,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>43</v>
@@ -2093,7 +2119,7 @@
         <v>24</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K43" s="7"/>
     </row>
@@ -2102,19 +2128,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>22</v>
@@ -2126,13 +2152,16 @@
         <v>24</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K44" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K19" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
EKA  TFT URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EARGE8PC\Desktop\btk42GithubIo\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2671244F-D664-4872-8D89-300B88C0A7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="92">
   <si>
     <t>Sıra</t>
   </si>
@@ -297,12 +298,15 @@
   </si>
   <si>
     <t>https://github.com/btk42/DP-D19-3X-000-LOP-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-EKA-TF-ACM-COP-S2B1-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -379,10 +383,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -673,1495 +676,1498 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="49.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="56.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="7"/>
+      <c r="J2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="7"/>
+      <c r="J3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="7"/>
+      <c r="H4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" s="7"/>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K6" s="7"/>
+      <c r="J6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K7" s="7"/>
+      <c r="J7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="6" t="s">
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" s="7"/>
+      <c r="J8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" s="7"/>
+      <c r="J9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="7"/>
+      <c r="J10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="6" t="s">
+      <c r="F11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="7"/>
+      <c r="J11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="F12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="7"/>
+      <c r="H12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="7"/>
+      <c r="H13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K14" s="7"/>
+      <c r="F14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K15" s="7"/>
+      <c r="I15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="6" t="s">
+      <c r="F16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="7"/>
+      <c r="I16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="6" t="s">
+      <c r="E17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K17" s="7"/>
+      <c r="H17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="7"/>
+      <c r="H18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="8" t="s">
+      <c r="E19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="6" t="s">
+      <c r="E20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="8" t="s">
+      <c r="I20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="6" t="s">
+      <c r="E21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K21" s="7"/>
+      <c r="I21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K22" s="8" t="s">
+      <c r="H22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="F23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K23" s="7"/>
+      <c r="H23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K24" s="7"/>
+      <c r="H24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="F25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K25" s="7"/>
+      <c r="H25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="6" t="s">
+      <c r="E26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K26" s="7"/>
+      <c r="H26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="6" t="s">
+      <c r="F27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K27" s="7"/>
+      <c r="H27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K28" s="7"/>
+      <c r="I28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="6" t="s">
+      <c r="E29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K29" s="7"/>
+      <c r="I29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="6" t="s">
+      <c r="E30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="6" t="s">
+      <c r="G30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K30" s="7"/>
+      <c r="I30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="6" t="s">
+      <c r="F31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K31" s="7"/>
+      <c r="H31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K32" s="7"/>
+      <c r="H32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K32" s="6"/>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="6" t="s">
+      <c r="E33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K33" s="7"/>
+      <c r="G33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="6"/>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="6" t="s">
+      <c r="E34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="6" t="s">
+      <c r="G34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K34" s="7"/>
+      <c r="J34" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="6"/>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="6" t="s">
+      <c r="E35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="6" t="s">
+      <c r="G35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K35" s="7"/>
+      <c r="J35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K35" s="6"/>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="6" t="s">
+      <c r="E36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K36" s="7"/>
+      <c r="G36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K36" s="6"/>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="6" t="s">
+      <c r="E37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="G37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I37" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K37" s="7"/>
+      <c r="I37" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="6" t="s">
+      <c r="G38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I38" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K38" s="7"/>
+      <c r="I38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K38" s="6"/>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="6" t="s">
+      <c r="E39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K39" s="7"/>
+      <c r="G39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K39" s="6"/>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="6" t="s">
+      <c r="E40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" s="6" t="s">
+      <c r="G40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I40" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K40" s="7"/>
+      <c r="I40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K40" s="6"/>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K41" s="7"/>
+      <c r="H41" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K41" s="6"/>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K42" s="7"/>
+      <c r="G42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K42" s="6"/>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G43" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K43" s="7"/>
+      <c r="I43" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K43" s="6"/>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F44" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="G44" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K44" s="7"/>
+      <c r="H44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K19" r:id="rId1"/>
+    <hyperlink ref="K19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K44" r:id="rId2" xr:uid="{37D72335-1EDA-4826-9B6A-206A46DA2199}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
T113i_T507_ESP32_Media_Player dosyası için kod oluşturuldu ve URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2671244F-D664-4872-8D89-300B88C0A7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA974567-A8DE-46E2-AA5D-871771A57108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="95">
   <si>
     <t>Sıra</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>https://github.com/btk42/DP-EKA-TF-ACM-COP-S2B1-01</t>
+  </si>
+  <si>
+    <t>Model-02</t>
+  </si>
+  <si>
+    <t>DP-000-TF-RNS-CLI-H3B1-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-TF-RNS-CLI-H3B1-02</t>
   </si>
 </sst>
 </file>
@@ -679,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2098,7 +2107,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>60</v>
@@ -2122,9 +2131,11 @@
         <v>24</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="K43" s="6"/>
+        <v>92</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
@@ -2165,9 +2176,10 @@
   <hyperlinks>
     <hyperlink ref="K19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K44" r:id="rId2" xr:uid="{37D72335-1EDA-4826-9B6A-206A46DA2199}"/>
+    <hyperlink ref="K43" r:id="rId3" xr:uid="{93E664BD-8E26-4D85-AF3C-8EDAD9A4C0BD}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Göstergelerdeki TFT projelerinden 2 sinin proje kodu güncellendi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA974567-A8DE-46E2-AA5D-871771A57108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE1FB07-BC19-4058-8493-3549F55183CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -204,9 +204,6 @@
     <t>DP-PNT-3X-RNS-LOP-S2B1-01</t>
   </si>
   <si>
-    <t>DP-000-TF-RNS-CLI-H3B1-01</t>
-  </si>
-  <si>
     <t>Bağımsız Tasarım</t>
   </si>
   <si>
@@ -306,10 +303,13 @@
     <t>Model-02</t>
   </si>
   <si>
-    <t>DP-000-TF-RNS-CLI-H3B1-02</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/DP-000-TF-RNS-CLI-H3B1-02</t>
+    <t>DP-000-TF-ACM-CLI-H3B1-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-TF-ACM-CLI-H3B1-02</t>
+  </si>
+  <si>
+    <t>DP-000-TF-ACM-CLI-H3B1-01</t>
   </si>
 </sst>
 </file>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -698,7 +698,7 @@
     <col min="2" max="2" width="28.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" style="3" customWidth="1"/>
     <col min="6" max="6" width="18.109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" style="3" customWidth="1"/>
@@ -772,7 +772,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K2" s="6"/>
     </row>
@@ -805,7 +805,7 @@
         <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -838,7 +838,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -871,7 +871,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -904,7 +904,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -937,7 +937,7 @@
         <v>18</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -970,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1003,7 +1003,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -1036,7 +1036,7 @@
         <v>18</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="6"/>
     </row>
@@ -1069,7 +1069,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1102,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="6"/>
     </row>
@@ -1135,7 +1135,7 @@
         <v>24</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1168,7 +1168,7 @@
         <v>24</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" s="6"/>
     </row>
@@ -1201,7 +1201,7 @@
         <v>24</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1234,7 +1234,7 @@
         <v>24</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K16" s="6"/>
     </row>
@@ -1246,7 +1246,7 @@
         <v>45</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>46</v>
@@ -1267,7 +1267,7 @@
         <v>24</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1279,7 +1279,7 @@
         <v>47</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>46</v>
@@ -1300,7 +1300,7 @@
         <v>24</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -1309,7 +1309,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>33</v>
@@ -1333,10 +1333,10 @@
         <v>24</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1344,7 +1344,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>33</v>
@@ -1368,10 +1368,10 @@
         <v>24</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1403,7 +1403,7 @@
         <v>24</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -1436,10 +1436,10 @@
         <v>24</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1471,7 +1471,7 @@
         <v>24</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K23" s="6"/>
     </row>
@@ -1504,7 +1504,7 @@
         <v>24</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -1537,7 +1537,7 @@
         <v>24</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -1570,7 +1570,7 @@
         <v>24</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K26" s="6"/>
     </row>
@@ -1603,7 +1603,7 @@
         <v>24</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K27" s="6"/>
     </row>
@@ -1612,22 +1612,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>43</v>
@@ -1636,7 +1636,7 @@
         <v>24</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K28" s="6"/>
     </row>
@@ -1645,13 +1645,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>14</v>
@@ -1669,7 +1669,7 @@
         <v>24</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K29" s="6"/>
     </row>
@@ -1678,19 +1678,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>16</v>
@@ -1702,7 +1702,7 @@
         <v>24</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K30" s="6"/>
     </row>
@@ -1711,13 +1711,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
@@ -1735,7 +1735,7 @@
         <v>24</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K31" s="6"/>
     </row>
@@ -1744,19 +1744,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>22</v>
@@ -1768,7 +1768,7 @@
         <v>24</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1777,20 +1777,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="G33" s="5" t="s">
         <v>16</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>24</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K33" s="6"/>
     </row>
@@ -1810,19 +1810,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="E34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>16</v>
@@ -1834,7 +1834,7 @@
         <v>18</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K34" s="6"/>
     </row>
@@ -1843,19 +1843,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>16</v>
@@ -1867,7 +1867,7 @@
         <v>18</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K35" s="6"/>
     </row>
@@ -1876,7 +1876,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>33</v>
@@ -1888,7 +1888,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>16</v>
@@ -1900,7 +1900,7 @@
         <v>24</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K36" s="6"/>
     </row>
@@ -1909,7 +1909,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>33</v>
@@ -1921,7 +1921,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>16</v>
@@ -1933,7 +1933,7 @@
         <v>24</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K37" s="6"/>
     </row>
@@ -1942,7 +1942,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>33</v>
@@ -1954,7 +1954,7 @@
         <v>27</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>16</v>
@@ -1966,7 +1966,7 @@
         <v>24</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K38" s="6"/>
     </row>
@@ -1975,7 +1975,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>33</v>
@@ -1987,7 +1987,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>16</v>
@@ -1999,7 +1999,7 @@
         <v>24</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K39" s="6"/>
     </row>
@@ -2008,7 +2008,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>33</v>
@@ -2020,7 +2020,7 @@
         <v>14</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>16</v>
@@ -2032,7 +2032,7 @@
         <v>24</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K40" s="6"/>
     </row>
@@ -2041,7 +2041,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>33</v>
@@ -2053,7 +2053,7 @@
         <v>54</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>22</v>
@@ -2065,7 +2065,7 @@
         <v>24</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K41" s="6"/>
     </row>
@@ -2074,7 +2074,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>33</v>
@@ -2086,7 +2086,7 @@
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>16</v>
@@ -2098,7 +2098,7 @@
         <v>24</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K42" s="6"/>
     </row>
@@ -2107,22 +2107,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="E43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F43" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>43</v>
@@ -2131,10 +2131,10 @@
         <v>24</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2142,19 +2142,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>22</v>
@@ -2166,10 +2166,10 @@
         <v>24</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
linkleri ilk git kaldırma
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE1FB07-BC19-4058-8493-3549F55183CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B0556C-ED86-46F7-9D9F-458A05FF7882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35805" yWindow="0" windowWidth="21225" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="109">
   <si>
     <t>Sıra</t>
   </si>
@@ -310,6 +310,48 @@
   </si>
   <si>
     <t>DP-000-TF-ACM-CLI-H3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-EKO-7S-000-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-HBT-7S-000-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-000-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-000-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-000-LOP-P2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-000-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-GLX-7S-000-LOP-P2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-GLX-7S-000-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>Yakamoz</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-YKZ-7S-000-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>DP-YKZ-7S-000-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>DP-YKZ-7S-000-LOP-P2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-YKZ-7S-000-LOP-P2B0-01</t>
   </si>
 </sst>
 </file>
@@ -392,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -403,7 +445,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -686,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -774,7 +815,9 @@
       <c r="J2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -807,7 +850,9 @@
       <c r="J3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
@@ -840,7 +885,9 @@
       <c r="J4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
@@ -873,7 +920,9 @@
       <c r="J5" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
@@ -906,7 +955,9 @@
       <c r="J6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
@@ -939,7 +990,9 @@
       <c r="J7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
@@ -972,7 +1025,9 @@
       <c r="J8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
@@ -1005,7 +1060,9 @@
       <c r="J9" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -1038,7 +1095,9 @@
       <c r="J10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -1071,7 +1130,9 @@
       <c r="J11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
@@ -1104,7 +1165,9 @@
       <c r="J12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
@@ -1137,7 +1200,9 @@
       <c r="J13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
@@ -1170,7 +1235,9 @@
       <c r="J14" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
@@ -1203,7 +1270,9 @@
       <c r="J15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
@@ -1236,7 +1305,9 @@
       <c r="J16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="6"/>
+      <c r="K16" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
@@ -1269,7 +1340,9 @@
       <c r="J17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="6"/>
+      <c r="K17" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
@@ -1302,7 +1375,9 @@
       <c r="J18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
@@ -1335,7 +1410,7 @@
       <c r="J19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="6" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1370,7 +1445,7 @@
       <c r="J20" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="6" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1405,7 +1480,9 @@
       <c r="J21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K21" s="6"/>
+      <c r="K21" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
@@ -1438,7 +1515,7 @@
       <c r="J22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="6" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1473,7 +1550,9 @@
       <c r="J23" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
@@ -1506,7 +1585,9 @@
       <c r="J24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
@@ -1539,7 +1620,9 @@
       <c r="J25" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K25" s="6"/>
+      <c r="K25" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
@@ -1572,7 +1655,9 @@
       <c r="J26" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K26" s="6"/>
+      <c r="K26" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
@@ -1605,7 +1690,9 @@
       <c r="J27" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K27" s="6"/>
+      <c r="K27" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
@@ -1638,7 +1725,9 @@
       <c r="J28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K28" s="6"/>
+      <c r="K28" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
@@ -1671,7 +1760,9 @@
       <c r="J29" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K29" s="6"/>
+      <c r="K29" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
@@ -1704,7 +1795,9 @@
       <c r="J30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K30" s="6"/>
+      <c r="K30" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
@@ -1737,7 +1830,9 @@
       <c r="J31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K31" s="6"/>
+      <c r="K31" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -1770,7 +1865,9 @@
       <c r="J32" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K32" s="6"/>
+      <c r="K32" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
@@ -1803,7 +1900,9 @@
       <c r="J33" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="6"/>
+      <c r="K33" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -1836,7 +1935,9 @@
       <c r="J34" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K34" s="6"/>
+      <c r="K34" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -1869,7 +1970,9 @@
       <c r="J35" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K35" s="6"/>
+      <c r="K35" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
@@ -1902,7 +2005,9 @@
       <c r="J36" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K36" s="6"/>
+      <c r="K36" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -1935,7 +2040,9 @@
       <c r="J37" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K37" s="6"/>
+      <c r="K37" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
@@ -1968,7 +2075,9 @@
       <c r="J38" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K38" s="6"/>
+      <c r="K38" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
@@ -2001,7 +2110,9 @@
       <c r="J39" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K39" s="6"/>
+      <c r="K39" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
@@ -2034,7 +2145,9 @@
       <c r="J40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K40" s="6"/>
+      <c r="K40" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
@@ -2067,7 +2180,9 @@
       <c r="J41" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K41" s="6"/>
+      <c r="K41" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
@@ -2100,7 +2215,9 @@
       <c r="J42" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K42" s="6"/>
+      <c r="K42" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
@@ -2133,7 +2250,7 @@
       <c r="J43" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K43" s="7" t="s">
+      <c r="K43" s="6" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2168,8 +2285,78 @@
       <c r="J44" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K44" s="7" t="s">
+      <c r="K44" s="6" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2177,9 +2364,24 @@
     <hyperlink ref="K19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K44" r:id="rId2" xr:uid="{37D72335-1EDA-4826-9B6A-206A46DA2199}"/>
     <hyperlink ref="K43" r:id="rId3" xr:uid="{93E664BD-8E26-4D85-AF3C-8EDAD9A4C0BD}"/>
+    <hyperlink ref="K2" r:id="rId4" xr:uid="{B6E3A22D-569A-4BCB-9A79-2E0B5E3CB3E5}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{673D7073-4F14-475B-A619-4618DD3FBC71}"/>
+    <hyperlink ref="K4" r:id="rId6" xr:uid="{E5B3FD63-EB5F-49BB-A0FC-A463CCC4535D}"/>
+    <hyperlink ref="K5:K18" r:id="rId7" display="https://github.com/btk42/DP-" xr:uid="{5A0C3DD0-DBEB-4BD5-AFDA-6D33D12D5B09}"/>
+    <hyperlink ref="K21" r:id="rId8" xr:uid="{233AC934-3708-444B-A94E-0E3FB27F6683}"/>
+    <hyperlink ref="K23" r:id="rId9" xr:uid="{03A7099B-7754-4020-957F-46712634C8F7}"/>
+    <hyperlink ref="K24:K42" r:id="rId10" display="https://github.com/btk42/DP-" xr:uid="{4B809462-F841-4726-8C97-412FB3C48871}"/>
+    <hyperlink ref="K6" r:id="rId11" xr:uid="{6EA7C7CB-B9FA-41DF-82FC-ABC696634AB1}"/>
+    <hyperlink ref="K36" r:id="rId12" xr:uid="{72FA59AA-C508-44EF-9DDB-B3C328C81638}"/>
+    <hyperlink ref="K37" r:id="rId13" xr:uid="{0A5FC444-8C8C-4A62-9126-A776D0D01AC5}"/>
+    <hyperlink ref="K10" r:id="rId14" xr:uid="{17D3C3E8-7B7B-42CB-8B02-EA2D1F2E37F2}"/>
+    <hyperlink ref="K9" r:id="rId15" xr:uid="{60D56623-7649-4DC1-BF34-AE510A15758C}"/>
+    <hyperlink ref="K8" r:id="rId16" xr:uid="{2FD48F14-AEA1-43F6-BB70-13A4DEC002DF}"/>
+    <hyperlink ref="K45" r:id="rId17" xr:uid="{EFE7F8D9-5DDE-4E5B-888B-1F2991BE26CB}"/>
+    <hyperlink ref="K46" r:id="rId18" xr:uid="{825E1A0F-E7F5-42B3-A8C3-AFA9720F4E33}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
2 Oklar ayrı paralel Dot projesinin kodu ve urls  eklendi. (DP-000-2D-NUV-LIP-P2B1-01)
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B0556C-ED86-46F7-9D9F-458A05FF7882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7444E1-8BB7-4F93-B085-963C5140739F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35805" yWindow="0" windowWidth="21225" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="111">
   <si>
     <t>Sıra</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>https://github.com/btk42/DP-YKZ-7S-000-LOP-P2B0-01</t>
+  </si>
+  <si>
+    <t>DP-000-2D-NUV-LIP-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-2D-NUV-LIP-P2B1-01</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -446,6 +452,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -727,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2290,13 +2297,13 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3">
+      <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="7" t="s">
         <v>104</v>
       </c>
       <c r="D45" s="5" t="s">
@@ -2325,13 +2332,13 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3">
+      <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="7" t="s">
         <v>104</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -2357,6 +2364,41 @@
       </c>
       <c r="K46" s="6" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2379,9 +2421,10 @@
     <hyperlink ref="K8" r:id="rId16" xr:uid="{2FD48F14-AEA1-43F6-BB70-13A4DEC002DF}"/>
     <hyperlink ref="K45" r:id="rId17" xr:uid="{EFE7F8D9-5DDE-4E5B-888B-1F2991BE26CB}"/>
     <hyperlink ref="K46" r:id="rId18" xr:uid="{825E1A0F-E7F5-42B3-A8C3-AFA9720F4E33}"/>
+    <hyperlink ref="K47" r:id="rId19" xr:uid="{A1BDA74E-1F9A-4061-B250-267EFC06F2CC}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
1 önceki commit düzenlendi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7444E1-8BB7-4F93-B085-963C5140739F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D91206C-E5EE-4B9D-B5D6-52D14F40DB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="112">
   <si>
     <t>Sıra</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/DP-000-2D-NUV-LIP-P2B1-01</t>
+  </si>
+  <si>
+    <t>2 Oklu Dot</t>
   </si>
 </sst>
 </file>
@@ -737,7 +740,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2377,7 +2380,7 @@
         <v>59</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
"DP-D19-DT-2OK-LIP-S2B1-01" ifadesi "DP-D19-2D-ACM-LIP-S2B1-01" olarak güncellendi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Depom\Projects\_GithubIO\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D91206C-E5EE-4B9D-B5D6-52D14F40DB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFBDD3F-DAE1-4D88-9671-1572B1483A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="111">
   <si>
     <t>Sıra</t>
   </si>
@@ -177,12 +177,6 @@
     <t>DP-PNT-3X-000-LOP-P3B1-01</t>
   </si>
   <si>
-    <t>DP-D19-DT-2OK-LIP-S2B1-01</t>
-  </si>
-  <si>
-    <t>2 Oklu 3x Dot</t>
-  </si>
-  <si>
     <t>RNS+Nuvo Mcu</t>
   </si>
   <si>
@@ -282,9 +276,6 @@
     <t>EKA</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-D19-DT-2OK-LIP-S2B1-01.git</t>
-  </si>
-  <si>
     <t>DP-D19-3X-000-LOP-P2B1-01</t>
   </si>
   <si>
@@ -361,6 +352,12 @@
   </si>
   <si>
     <t>2 Oklu Dot</t>
+  </si>
+  <si>
+    <t>DP-D19-2D-ACM-LIP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-2D-ACM-LIP-S2B1-01</t>
   </si>
 </sst>
 </file>
@@ -739,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -748,7 +745,7 @@
     <col min="1" max="1" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" style="3" customWidth="1"/>
     <col min="6" max="6" width="18.109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" style="3" customWidth="1"/>
@@ -823,10 +820,10 @@
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -858,10 +855,10 @@
         <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -893,10 +890,10 @@
         <v>24</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -928,10 +925,10 @@
         <v>24</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -963,10 +960,10 @@
         <v>18</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -998,10 +995,10 @@
         <v>18</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1033,10 +1030,10 @@
         <v>18</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1068,10 +1065,10 @@
         <v>18</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1103,10 +1100,10 @@
         <v>18</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1138,10 +1135,10 @@
         <v>18</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1173,10 +1170,10 @@
         <v>24</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1208,10 +1205,10 @@
         <v>24</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1243,10 +1240,10 @@
         <v>24</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1278,10 +1275,10 @@
         <v>24</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1313,10 +1310,10 @@
         <v>24</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1327,7 +1324,7 @@
         <v>45</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>46</v>
@@ -1348,10 +1345,10 @@
         <v>24</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1362,7 +1359,7 @@
         <v>47</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>46</v>
@@ -1383,10 +1380,10 @@
         <v>24</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1394,7 +1391,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>33</v>
@@ -1418,10 +1415,10 @@
         <v>24</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1429,7 +1426,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>33</v>
@@ -1453,10 +1450,10 @@
         <v>24</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1488,10 +1485,10 @@
         <v>24</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1499,16 +1496,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>39</v>
@@ -1523,10 +1520,10 @@
         <v>24</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1534,7 +1531,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>33</v>
@@ -1543,7 +1540,7 @@
         <v>48</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>15</v>
@@ -1558,10 +1555,10 @@
         <v>24</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1569,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>33</v>
@@ -1578,7 +1575,7 @@
         <v>48</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>39</v>
@@ -1593,10 +1590,10 @@
         <v>24</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1604,7 +1601,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>33</v>
@@ -1628,10 +1625,10 @@
         <v>24</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1639,7 +1636,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>42</v>
@@ -1663,10 +1660,10 @@
         <v>24</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1674,7 +1671,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>42</v>
@@ -1698,10 +1695,10 @@
         <v>24</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1709,22 +1706,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>43</v>
@@ -1733,10 +1730,10 @@
         <v>24</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1744,13 +1741,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>14</v>
@@ -1768,10 +1765,10 @@
         <v>24</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1779,19 +1776,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>16</v>
@@ -1803,10 +1800,10 @@
         <v>24</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1814,13 +1811,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>37</v>
@@ -1838,10 +1835,10 @@
         <v>24</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1849,19 +1846,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>22</v>
@@ -1873,10 +1870,10 @@
         <v>24</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1884,20 +1881,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="G33" s="5" t="s">
         <v>16</v>
       </c>
@@ -1908,10 +1905,10 @@
         <v>24</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1919,19 +1916,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="E34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>16</v>
@@ -1943,10 +1940,10 @@
         <v>18</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1954,19 +1951,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>16</v>
@@ -1978,10 +1975,10 @@
         <v>18</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1989,7 +1986,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>33</v>
@@ -2001,7 +1998,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>16</v>
@@ -2013,10 +2010,10 @@
         <v>24</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2024,7 +2021,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>33</v>
@@ -2036,7 +2033,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>16</v>
@@ -2048,10 +2045,10 @@
         <v>24</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2059,7 +2056,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>33</v>
@@ -2071,7 +2068,7 @@
         <v>27</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>16</v>
@@ -2083,10 +2080,10 @@
         <v>24</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2094,7 +2091,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>33</v>
@@ -2106,7 +2103,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>16</v>
@@ -2118,10 +2115,10 @@
         <v>24</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2129,7 +2126,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>33</v>
@@ -2141,7 +2138,7 @@
         <v>14</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>16</v>
@@ -2153,10 +2150,10 @@
         <v>24</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2164,7 +2161,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>33</v>
@@ -2173,10 +2170,10 @@
         <v>48</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>22</v>
@@ -2188,10 +2185,10 @@
         <v>24</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2199,7 +2196,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>33</v>
@@ -2211,7 +2208,7 @@
         <v>37</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>16</v>
@@ -2223,10 +2220,10 @@
         <v>24</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2234,22 +2231,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>43</v>
@@ -2258,10 +2255,10 @@
         <v>24</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2269,19 +2266,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>22</v>
@@ -2293,10 +2290,10 @@
         <v>24</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2304,10 +2301,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>13</v>
@@ -2328,10 +2325,10 @@
         <v>18</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2339,10 +2336,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>13</v>
@@ -2363,10 +2360,10 @@
         <v>18</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2374,16 +2371,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>39</v>
@@ -2398,10 +2395,10 @@
         <v>24</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2425,9 +2422,10 @@
     <hyperlink ref="K45" r:id="rId17" xr:uid="{EFE7F8D9-5DDE-4E5B-888B-1F2991BE26CB}"/>
     <hyperlink ref="K46" r:id="rId18" xr:uid="{825E1A0F-E7F5-42B3-A8C3-AFA9720F4E33}"/>
     <hyperlink ref="K47" r:id="rId19" xr:uid="{A1BDA74E-1F9A-4061-B250-267EFC06F2CC}"/>
+    <hyperlink ref="K22" r:id="rId20" xr:uid="{8F438F7F-6F3C-435B-8C66-89BE2696B903}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Gösterge Kodlar düzeltilip, linkler eklendi
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Depom\Projects\_GithubIO\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFBDD3F-DAE1-4D88-9671-1572B1483A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02FF01-B7EC-42CE-8D94-F93D2BC6F2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="140">
   <si>
     <t>Sıra</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Hobbit</t>
   </si>
   <si>
-    <t>DP-HBT-7S-000-LOP-S2B1-01</t>
-  </si>
-  <si>
     <t>Seri</t>
   </si>
   <si>
@@ -219,12 +216,6 @@
     <t>DP-000-LC-000-CLI-P1B1-01</t>
   </si>
   <si>
-    <t>DP-000-LC-RNS-LOP-S2B1-01</t>
-  </si>
-  <si>
-    <t>DP-000-LC-RNS-CLI-S2B1-01</t>
-  </si>
-  <si>
     <t>DP-000-TF-000-CLI-P2B1-01</t>
   </si>
   <si>
@@ -303,9 +294,6 @@
     <t>DP-000-TF-ACM-CLI-H3B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/DP-EKO-7S-000-LOP-P1B0-01</t>
   </si>
   <si>
@@ -358,6 +346,105 @@
   </si>
   <si>
     <t>https://github.com/btk42/DP-D19-2D-ACM-LIP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-RNS-LIP-S2B1-01</t>
+  </si>
+  <si>
+    <t>DP-HBT-7S-RNS-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-HBT-7S-RNS-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-GLX-7S-BIN-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-GLX-7S-GRY-LOP-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-BIN-LOP-P1B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-RNS-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-GRY-LOP-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-PNT-7S-000-LOP-P3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-PNT-7S-BIN-LOP-P3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-EKA-DT-000-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-EKA-DT-000-LIP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-PNT-3X-000-LOP-P3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-NUV-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-NUV-LIP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-RNS-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-PNT-3X-000-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-PNT-3X-RNS-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-TF-ACM-CLI-H3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-LC-000-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-LC-000-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>DP-000-LC-ACM-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>DP-000-LC-ACM-CLI-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-LC-ACM-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-LC-ACM-CLI-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-TF-000-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-B18-OK-000-CLI-P3B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-OK-000-000-P3B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-7S-GRY-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-000-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-000-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-NUV-CLI-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-RNS-CLI-P2B1-01</t>
   </si>
 </sst>
 </file>
@@ -736,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -820,10 +907,10 @@
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -855,10 +942,10 @@
         <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -866,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>20</v>
@@ -875,25 +962,25 @@
         <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -901,16 +988,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>15</v>
@@ -919,16 +1006,16 @@
         <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -936,10 +1023,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>13</v>
@@ -954,16 +1041,16 @@
         <v>16</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -971,16 +1058,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>15</v>
@@ -995,10 +1082,10 @@
         <v>18</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1006,10 +1093,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>13</v>
@@ -1030,10 +1117,10 @@
         <v>18</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1041,10 +1128,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>13</v>
@@ -1065,10 +1152,10 @@
         <v>18</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1076,10 +1163,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>13</v>
@@ -1094,16 +1181,16 @@
         <v>16</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1111,16 +1198,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>15</v>
@@ -1135,10 +1222,10 @@
         <v>18</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1146,34 +1233,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1181,34 +1268,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1216,16 +1303,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>15</v>
@@ -1234,16 +1321,16 @@
         <v>16</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1251,10 +1338,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>13</v>
@@ -1269,16 +1356,16 @@
         <v>16</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1286,16 +1373,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>15</v>
@@ -1304,16 +1391,16 @@
         <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1321,13 +1408,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>14</v>
@@ -1336,19 +1423,19 @@
         <v>15</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1356,34 +1443,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1391,13 +1478,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>14</v>
@@ -1409,16 +1496,16 @@
         <v>16</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1426,13 +1513,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>14</v>
@@ -1447,13 +1534,13 @@
         <v>17</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1461,13 +1548,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>14</v>
@@ -1479,16 +1566,16 @@
         <v>16</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1496,34 +1583,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1531,34 +1618,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="F23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1566,34 +1653,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1601,34 +1688,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1636,13 +1723,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>14</v>
@@ -1651,19 +1738,19 @@
         <v>15</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1671,34 +1758,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1706,34 +1793,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H28" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1741,13 +1828,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>14</v>
@@ -1762,13 +1849,13 @@
         <v>17</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1776,19 +1863,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>16</v>
@@ -1797,13 +1884,13 @@
         <v>17</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1811,34 +1898,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1846,34 +1933,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1881,34 +1968,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1916,34 +2003,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1951,34 +2038,34 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1986,10 +2073,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>13</v>
@@ -1998,22 +2085,22 @@
         <v>14</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2021,10 +2108,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>13</v>
@@ -2033,7 +2120,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>16</v>
@@ -2042,13 +2129,13 @@
         <v>17</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2056,19 +2143,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>16</v>
@@ -2077,13 +2164,13 @@
         <v>17</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2091,34 +2178,34 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2126,19 +2213,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>16</v>
@@ -2147,13 +2234,13 @@
         <v>17</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2161,34 +2248,34 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2196,34 +2283,34 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2231,34 +2318,34 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="E43" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H43" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2266,34 +2353,34 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2301,10 +2388,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>13</v>
@@ -2325,10 +2412,10 @@
         <v>18</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2336,10 +2423,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>13</v>
@@ -2354,16 +2441,16 @@
         <v>16</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2371,34 +2458,34 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2423,9 +2510,36 @@
     <hyperlink ref="K46" r:id="rId18" xr:uid="{825E1A0F-E7F5-42B3-A8C3-AFA9720F4E33}"/>
     <hyperlink ref="K47" r:id="rId19" xr:uid="{A1BDA74E-1F9A-4061-B250-267EFC06F2CC}"/>
     <hyperlink ref="K22" r:id="rId20" xr:uid="{8F438F7F-6F3C-435B-8C66-89BE2696B903}"/>
+    <hyperlink ref="K13" r:id="rId21" xr:uid="{0177384F-6523-4648-AC4B-2457E215475A}"/>
+    <hyperlink ref="K5" r:id="rId22" xr:uid="{3DE1BB94-44BB-4DA1-B9A0-E70513C7CAAE}"/>
+    <hyperlink ref="K7" r:id="rId23" xr:uid="{C78259F8-B994-4ABD-A948-C1F170A5889C}"/>
+    <hyperlink ref="K11" r:id="rId24" xr:uid="{7D71F460-386D-49DD-A26B-672C1131433E}"/>
+    <hyperlink ref="K12" r:id="rId25" xr:uid="{A19AFFA6-7891-4FAB-B1B5-F2F0DB739CDB}"/>
+    <hyperlink ref="K14" r:id="rId26" xr:uid="{3904E34F-58FF-4343-8FDC-3C05315260FF}"/>
+    <hyperlink ref="K15" r:id="rId27" xr:uid="{2EBBC1C0-3B47-410C-AB78-4FD95CE4A46C}"/>
+    <hyperlink ref="K16" r:id="rId28" xr:uid="{1991491E-7812-44F1-A7DF-4969E1F5260D}"/>
+    <hyperlink ref="K17" r:id="rId29" xr:uid="{79076E3C-D40F-4409-BA26-5104B084A2F5}"/>
+    <hyperlink ref="K18" r:id="rId30" xr:uid="{D9CAFB21-EFF8-4540-80F1-3255EA4B50E2}"/>
+    <hyperlink ref="K24" r:id="rId31" xr:uid="{00637B7B-C732-4F2B-91D6-312897407376}"/>
+    <hyperlink ref="K25" r:id="rId32" xr:uid="{A4239629-4E71-4599-BD09-8FBA646E6D20}"/>
+    <hyperlink ref="K26" r:id="rId33" xr:uid="{EE418F3E-6631-4295-9897-11D5C18E87D6}"/>
+    <hyperlink ref="K27" r:id="rId34" xr:uid="{97396C99-0023-426B-8BAC-29C6E0ED9367}"/>
+    <hyperlink ref="K28" r:id="rId35" xr:uid="{27477871-03E5-4042-8D08-1D3783C73515}"/>
+    <hyperlink ref="K29" r:id="rId36" xr:uid="{1D91FD5E-8C31-4158-A00C-1A34FC5C1AEC}"/>
+    <hyperlink ref="K30" r:id="rId37" xr:uid="{4BAB16A3-12E5-43E8-A342-E76C738C6DA6}"/>
+    <hyperlink ref="K31" r:id="rId38" xr:uid="{74EF131F-4098-458F-A36A-9EC85328F4DC}"/>
+    <hyperlink ref="K32" r:id="rId39" xr:uid="{9E17C17B-C6B1-4427-86EE-AD0662111F11}"/>
+    <hyperlink ref="K33" r:id="rId40" xr:uid="{02612884-0E8F-4E02-BC26-D05308DAF5A3}"/>
+    <hyperlink ref="K34" r:id="rId41" xr:uid="{F6D5B895-61F4-4038-8BF9-195A16A4538A}"/>
+    <hyperlink ref="K35" r:id="rId42" xr:uid="{4278A311-C1EA-4D50-B4BA-ABA7AF84FF25}"/>
+    <hyperlink ref="K38" r:id="rId43" xr:uid="{A8A7BC6C-429E-429E-8029-B8F174C52A38}"/>
+    <hyperlink ref="K39" r:id="rId44" xr:uid="{37F27EA4-F903-4349-905D-75AC5C72F0AF}"/>
+    <hyperlink ref="K40" r:id="rId45" xr:uid="{E1D98A40-A546-4008-97BF-13BE3516D00B}"/>
+    <hyperlink ref="K41" r:id="rId46" xr:uid="{65B8D420-0E76-4D63-9F29-041A679C3411}"/>
+    <hyperlink ref="K42" r:id="rId47" xr:uid="{6C46F972-3E8C-4F4B-B90D-53BABED3FBE0}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId48"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Gösterge Nuvoton ve ACM kod eksiklikleri giderildi
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02FF01-B7EC-42CE-8D94-F93D2BC6F2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7074CD6-D5A4-4962-B21A-D6988FFDD039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="143">
   <si>
     <t>Sıra</t>
   </si>
@@ -159,21 +159,12 @@
     <t>DP-PNT-7S-BIN-LOP-P3B1-01</t>
   </si>
   <si>
-    <t>DP-EKA-DT-000-LOP-S2B1-01</t>
-  </si>
-  <si>
     <t>Bağımsız Dot</t>
   </si>
   <si>
-    <t>DP-EKA-DT-000-LIP-S2B1-01</t>
-  </si>
-  <si>
     <t>3x Dot</t>
   </si>
   <si>
-    <t>DP-PNT-3X-000-LOP-P3B1-01</t>
-  </si>
-  <si>
     <t>RNS+Nuvo Mcu</t>
   </si>
   <si>
@@ -189,9 +180,6 @@
     <t>DP-D19-3X-RNS-LOP-S2B1-01</t>
   </si>
   <si>
-    <t>DP-PNT-3X-000-LOP-S2B1-01</t>
-  </si>
-  <si>
     <t>DP-PNT-3X-RNS-LOP-S2B1-01</t>
   </si>
   <si>
@@ -207,18 +195,9 @@
     <t>Seri&amp;Paralel</t>
   </si>
   <si>
-    <t>DP-000-LC-000-LOP-P1B1-01</t>
-  </si>
-  <si>
     <t>LCD</t>
   </si>
   <si>
-    <t>DP-000-LC-000-CLI-P1B1-01</t>
-  </si>
-  <si>
-    <t>DP-000-TF-000-CLI-P2B1-01</t>
-  </si>
-  <si>
     <t>DP-B18-OK-000-CLI-P3B0-01</t>
   </si>
   <si>
@@ -243,12 +222,6 @@
     <t>DP-D19-7S-GRY-CLI-P1B1-01</t>
   </si>
   <si>
-    <t>DP-D19-3X-000-CLI-P2B1-01</t>
-  </si>
-  <si>
-    <t>DP-D19-3X-000-CLI-P1B1-01</t>
-  </si>
-  <si>
     <t>DP-D19-3X-NUV-CLI-S2B1-01</t>
   </si>
   <si>
@@ -267,18 +240,6 @@
     <t>EKA</t>
   </si>
   <si>
-    <t>DP-D19-3X-000-LOP-P2B1-01</t>
-  </si>
-  <si>
-    <t>DP-D19-3X-000-LOP-P1B1-01</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/DP-D19-3X-000-LOP-P1B1-01</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/DP-D19-3X-000-LOP-P2B1-01</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/DP-EKA-TF-ACM-COP-S2B1-01</t>
   </si>
   <si>
@@ -378,15 +339,6 @@
     <t>https://github.com/btk42/DP-PNT-7S-BIN-LOP-P3B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-EKA-DT-000-LOP-S2B1-01</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/DP-EKA-DT-000-LIP-S2B1-01</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/DP-PNT-3X-000-LOP-P3B1-01</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/DP-D19-3X-NUV-LOP-S2B1-01</t>
   </si>
   <si>
@@ -396,21 +348,12 @@
     <t>https://github.com/btk42/DP-D19-3X-RNS-LOP-S2B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-PNT-3X-000-LOP-S2B1-01</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/DP-PNT-3X-RNS-LOP-S2B1-01</t>
   </si>
   <si>
     <t>https://github.com/btk42/DP-000-TF-ACM-CLI-H3B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-000-LC-000-LOP-P1B1-01</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/DP-000-LC-000-CLI-P1B1-01</t>
-  </si>
-  <si>
     <t>DP-000-LC-ACM-LOP-S2B1-01</t>
   </si>
   <si>
@@ -423,9 +366,6 @@
     <t>https://github.com/btk42/DP-000-LC-ACM-CLI-S2B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-000-TF-000-CLI-P2B1-01</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/DP-B18-OK-000-CLI-P3B0-01</t>
   </si>
   <si>
@@ -435,16 +375,85 @@
     <t>https://github.com/btk42/DP-D19-7S-GRY-CLI-P1B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-D19-3X-000-CLI-P2B1-01</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/DP-D19-3X-000-CLI-P1B1-01</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/DP-D19-3X-NUV-CLI-S2B1-01</t>
   </si>
   <si>
     <t>https://github.com/btk42/DP-D19-3X-RNS-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>2 Oklu 7Seg</t>
+  </si>
+  <si>
+    <t>DP-000-2S-000-LIP-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-2S-000-LIP-P2B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-3X-NUV-LOP-P2B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-3X-NUV-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>DP-PNT-3X-NUV-LOP-P3B1-01</t>
+  </si>
+  <si>
+    <t>DP-PNT-3X-NUV-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>DP-000-LC-NUV-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>DP-000-LC-NUV-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>DP-000-TF-NUV-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-3X-NUV-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-3X-NUV-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-NUV-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-PNT-3X-NUV-LOP-P3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/D19-3X-DP-NUV-LOP-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-PNT-3X-NUV-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-LC-NUV-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-LC-NUV-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-NUV-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-NUV-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-TF-NUV-CLI-P2B1-01</t>
+  </si>
+  <si>
+    <t>DP-EKA-DT-ACM-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>DP-EKA-DT-ACM-LIP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-EKA-DT-ACM-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-EKA-DT-ACM-LIP-S2B1-01</t>
   </si>
 </sst>
 </file>
@@ -491,12 +500,18 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -527,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -540,6 +555,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -821,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -907,10 +923,10 @@
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -942,10 +958,10 @@
         <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -953,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>20</v>
@@ -977,10 +993,10 @@
         <v>23</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1012,10 +1028,10 @@
         <v>23</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1047,10 +1063,10 @@
         <v>18</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1082,10 +1098,10 @@
         <v>18</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1117,10 +1133,10 @@
         <v>18</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1152,10 +1168,10 @@
         <v>18</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1187,10 +1203,10 @@
         <v>18</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1222,10 +1238,10 @@
         <v>18</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1257,10 +1273,10 @@
         <v>23</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1292,10 +1308,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1327,10 +1343,10 @@
         <v>23</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1362,10 +1378,10 @@
         <v>23</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1397,27 +1413,27 @@
         <v>23</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>15</v>
@@ -1432,27 +1448,28 @@
         <v>23</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>38</v>
@@ -1467,27 +1484,28 @@
         <v>23</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>15</v>
@@ -1502,27 +1520,27 @@
         <v>23</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>15</v>
@@ -1537,27 +1555,27 @@
         <v>23</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>15</v>
@@ -1572,27 +1590,27 @@
         <v>23</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>38</v>
@@ -1607,27 +1625,27 @@
         <v>23</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>15</v>
@@ -1642,27 +1660,27 @@
         <v>23</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>38</v>
@@ -1677,24 +1695,24 @@
         <v>23</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>36</v>
@@ -1712,27 +1730,27 @@
         <v>23</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>15</v>
@@ -1747,24 +1765,24 @@
         <v>23</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>36</v>
@@ -1782,33 +1800,33 @@
         <v>23</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>42</v>
@@ -1817,27 +1835,27 @@
         <v>23</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E29" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>15</v>
@@ -1852,30 +1870,30 @@
         <v>23</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E30" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>16</v>
@@ -1887,27 +1905,27 @@
         <v>23</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E31" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>15</v>
@@ -1922,30 +1940,30 @@
         <v>23</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E32" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>21</v>
@@ -1957,10 +1975,10 @@
         <v>23</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1968,19 +1986,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>16</v>
@@ -1992,10 +2010,10 @@
         <v>23</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2003,19 +2021,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>16</v>
@@ -2027,10 +2045,10 @@
         <v>18</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2038,19 +2056,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>16</v>
@@ -2062,10 +2080,10 @@
         <v>18</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2073,7 +2091,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>32</v>
@@ -2085,7 +2103,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>16</v>
@@ -2097,10 +2115,10 @@
         <v>23</v>
       </c>
       <c r="J36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2108,7 +2126,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>32</v>
@@ -2120,7 +2138,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>16</v>
@@ -2132,10 +2150,10 @@
         <v>23</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2143,7 +2161,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>32</v>
@@ -2155,7 +2173,7 @@
         <v>26</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>16</v>
@@ -2167,10 +2185,10 @@
         <v>23</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2178,19 +2196,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>16</v>
@@ -2202,10 +2220,10 @@
         <v>23</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2213,19 +2231,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>16</v>
@@ -2237,10 +2255,10 @@
         <v>23</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2248,19 +2266,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>21</v>
@@ -2272,10 +2290,10 @@
         <v>23</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2283,19 +2301,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>36</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>16</v>
@@ -2307,10 +2325,10 @@
         <v>23</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2318,22 +2336,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>42</v>
@@ -2342,10 +2360,10 @@
         <v>23</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2353,19 +2371,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>21</v>
@@ -2377,10 +2395,10 @@
         <v>23</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2388,10 +2406,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>13</v>
@@ -2412,10 +2430,10 @@
         <v>18</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2423,10 +2441,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>13</v>
@@ -2447,10 +2465,10 @@
         <v>18</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2458,16 +2476,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>38</v>
@@ -2482,10 +2500,45 @@
         <v>23</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>103</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2508,38 +2561,40 @@
     <hyperlink ref="K8" r:id="rId16" xr:uid="{2FD48F14-AEA1-43F6-BB70-13A4DEC002DF}"/>
     <hyperlink ref="K45" r:id="rId17" xr:uid="{EFE7F8D9-5DDE-4E5B-888B-1F2991BE26CB}"/>
     <hyperlink ref="K46" r:id="rId18" xr:uid="{825E1A0F-E7F5-42B3-A8C3-AFA9720F4E33}"/>
-    <hyperlink ref="K47" r:id="rId19" xr:uid="{A1BDA74E-1F9A-4061-B250-267EFC06F2CC}"/>
-    <hyperlink ref="K22" r:id="rId20" xr:uid="{8F438F7F-6F3C-435B-8C66-89BE2696B903}"/>
-    <hyperlink ref="K13" r:id="rId21" xr:uid="{0177384F-6523-4648-AC4B-2457E215475A}"/>
-    <hyperlink ref="K5" r:id="rId22" xr:uid="{3DE1BB94-44BB-4DA1-B9A0-E70513C7CAAE}"/>
-    <hyperlink ref="K7" r:id="rId23" xr:uid="{C78259F8-B994-4ABD-A948-C1F170A5889C}"/>
-    <hyperlink ref="K11" r:id="rId24" xr:uid="{7D71F460-386D-49DD-A26B-672C1131433E}"/>
-    <hyperlink ref="K12" r:id="rId25" xr:uid="{A19AFFA6-7891-4FAB-B1B5-F2F0DB739CDB}"/>
-    <hyperlink ref="K14" r:id="rId26" xr:uid="{3904E34F-58FF-4343-8FDC-3C05315260FF}"/>
-    <hyperlink ref="K15" r:id="rId27" xr:uid="{2EBBC1C0-3B47-410C-AB78-4FD95CE4A46C}"/>
-    <hyperlink ref="K16" r:id="rId28" xr:uid="{1991491E-7812-44F1-A7DF-4969E1F5260D}"/>
-    <hyperlink ref="K17" r:id="rId29" xr:uid="{79076E3C-D40F-4409-BA26-5104B084A2F5}"/>
-    <hyperlink ref="K18" r:id="rId30" xr:uid="{D9CAFB21-EFF8-4540-80F1-3255EA4B50E2}"/>
-    <hyperlink ref="K24" r:id="rId31" xr:uid="{00637B7B-C732-4F2B-91D6-312897407376}"/>
-    <hyperlink ref="K25" r:id="rId32" xr:uid="{A4239629-4E71-4599-BD09-8FBA646E6D20}"/>
-    <hyperlink ref="K26" r:id="rId33" xr:uid="{EE418F3E-6631-4295-9897-11D5C18E87D6}"/>
-    <hyperlink ref="K27" r:id="rId34" xr:uid="{97396C99-0023-426B-8BAC-29C6E0ED9367}"/>
-    <hyperlink ref="K28" r:id="rId35" xr:uid="{27477871-03E5-4042-8D08-1D3783C73515}"/>
-    <hyperlink ref="K29" r:id="rId36" xr:uid="{1D91FD5E-8C31-4158-A00C-1A34FC5C1AEC}"/>
-    <hyperlink ref="K30" r:id="rId37" xr:uid="{4BAB16A3-12E5-43E8-A342-E76C738C6DA6}"/>
-    <hyperlink ref="K31" r:id="rId38" xr:uid="{74EF131F-4098-458F-A36A-9EC85328F4DC}"/>
-    <hyperlink ref="K32" r:id="rId39" xr:uid="{9E17C17B-C6B1-4427-86EE-AD0662111F11}"/>
-    <hyperlink ref="K33" r:id="rId40" xr:uid="{02612884-0E8F-4E02-BC26-D05308DAF5A3}"/>
-    <hyperlink ref="K34" r:id="rId41" xr:uid="{F6D5B895-61F4-4038-8BF9-195A16A4538A}"/>
-    <hyperlink ref="K35" r:id="rId42" xr:uid="{4278A311-C1EA-4D50-B4BA-ABA7AF84FF25}"/>
-    <hyperlink ref="K38" r:id="rId43" xr:uid="{A8A7BC6C-429E-429E-8029-B8F174C52A38}"/>
-    <hyperlink ref="K39" r:id="rId44" xr:uid="{37F27EA4-F903-4349-905D-75AC5C72F0AF}"/>
-    <hyperlink ref="K40" r:id="rId45" xr:uid="{E1D98A40-A546-4008-97BF-13BE3516D00B}"/>
-    <hyperlink ref="K41" r:id="rId46" xr:uid="{65B8D420-0E76-4D63-9F29-041A679C3411}"/>
-    <hyperlink ref="K42" r:id="rId47" xr:uid="{6C46F972-3E8C-4F4B-B90D-53BABED3FBE0}"/>
+    <hyperlink ref="K22" r:id="rId19" xr:uid="{8F438F7F-6F3C-435B-8C66-89BE2696B903}"/>
+    <hyperlink ref="K13" r:id="rId20" xr:uid="{0177384F-6523-4648-AC4B-2457E215475A}"/>
+    <hyperlink ref="K5" r:id="rId21" xr:uid="{3DE1BB94-44BB-4DA1-B9A0-E70513C7CAAE}"/>
+    <hyperlink ref="K7" r:id="rId22" xr:uid="{C78259F8-B994-4ABD-A948-C1F170A5889C}"/>
+    <hyperlink ref="K11" r:id="rId23" xr:uid="{7D71F460-386D-49DD-A26B-672C1131433E}"/>
+    <hyperlink ref="K12" r:id="rId24" xr:uid="{A19AFFA6-7891-4FAB-B1B5-F2F0DB739CDB}"/>
+    <hyperlink ref="K14" r:id="rId25" xr:uid="{3904E34F-58FF-4343-8FDC-3C05315260FF}"/>
+    <hyperlink ref="K15" r:id="rId26" xr:uid="{2EBBC1C0-3B47-410C-AB78-4FD95CE4A46C}"/>
+    <hyperlink ref="K16" r:id="rId27" xr:uid="{1991491E-7812-44F1-A7DF-4969E1F5260D}"/>
+    <hyperlink ref="K17" r:id="rId28" xr:uid="{79076E3C-D40F-4409-BA26-5104B084A2F5}"/>
+    <hyperlink ref="K18" r:id="rId29" xr:uid="{D9CAFB21-EFF8-4540-80F1-3255EA4B50E2}"/>
+    <hyperlink ref="K24" r:id="rId30" xr:uid="{00637B7B-C732-4F2B-91D6-312897407376}"/>
+    <hyperlink ref="K25" r:id="rId31" xr:uid="{A4239629-4E71-4599-BD09-8FBA646E6D20}"/>
+    <hyperlink ref="K26" r:id="rId32" xr:uid="{EE418F3E-6631-4295-9897-11D5C18E87D6}"/>
+    <hyperlink ref="K27" r:id="rId33" xr:uid="{97396C99-0023-426B-8BAC-29C6E0ED9367}"/>
+    <hyperlink ref="K28" r:id="rId34" xr:uid="{27477871-03E5-4042-8D08-1D3783C73515}"/>
+    <hyperlink ref="K29" r:id="rId35" xr:uid="{1D91FD5E-8C31-4158-A00C-1A34FC5C1AEC}"/>
+    <hyperlink ref="K30" r:id="rId36" xr:uid="{4BAB16A3-12E5-43E8-A342-E76C738C6DA6}"/>
+    <hyperlink ref="K31" r:id="rId37" xr:uid="{74EF131F-4098-458F-A36A-9EC85328F4DC}"/>
+    <hyperlink ref="K32" r:id="rId38" xr:uid="{9E17C17B-C6B1-4427-86EE-AD0662111F11}"/>
+    <hyperlink ref="K33" r:id="rId39" xr:uid="{02612884-0E8F-4E02-BC26-D05308DAF5A3}"/>
+    <hyperlink ref="K34" r:id="rId40" xr:uid="{F6D5B895-61F4-4038-8BF9-195A16A4538A}"/>
+    <hyperlink ref="K35" r:id="rId41" xr:uid="{4278A311-C1EA-4D50-B4BA-ABA7AF84FF25}"/>
+    <hyperlink ref="K38" r:id="rId42" xr:uid="{A8A7BC6C-429E-429E-8029-B8F174C52A38}"/>
+    <hyperlink ref="K39" r:id="rId43" xr:uid="{37F27EA4-F903-4349-905D-75AC5C72F0AF}"/>
+    <hyperlink ref="K40" r:id="rId44" xr:uid="{E1D98A40-A546-4008-97BF-13BE3516D00B}"/>
+    <hyperlink ref="K41" r:id="rId45" xr:uid="{65B8D420-0E76-4D63-9F29-041A679C3411}"/>
+    <hyperlink ref="K42" r:id="rId46" xr:uid="{6C46F972-3E8C-4F4B-B90D-53BABED3FBE0}"/>
+    <hyperlink ref="K48" r:id="rId47" xr:uid="{D63EDBE2-BA4F-4AE1-AF14-7B86D2F69BDA}"/>
+    <hyperlink ref="K47" r:id="rId48" xr:uid="{A1BDA74E-1F9A-4061-B250-267EFC06F2CC}"/>
+    <hyperlink ref="K20" r:id="rId49" xr:uid="{E83A36DC-A6E2-4B10-8099-53E43FE4316B}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId48"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId50"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
2x dot kat kabin eklendi
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7074CD6-D5A4-4962-B21A-D6988FFDD039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137A4393-BA2E-4963-B7FF-9ED3A53613B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="148">
   <si>
     <t>Sıra</t>
   </si>
@@ -454,6 +454,21 @@
   </si>
   <si>
     <t>https://github.com/btk42/DP-EKA-DT-ACM-LIP-S2B1-01</t>
+  </si>
+  <si>
+    <t>2x Dot</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-2X-NUV-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-2X-NUV-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-2X-NUV-LOP-P1B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-2X-NUV-CLI-P1B1-01</t>
   </si>
 </sst>
 </file>
@@ -837,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2539,6 +2554,76 @@
       </c>
       <c r="K48" s="6" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>50</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2592,9 +2677,11 @@
     <hyperlink ref="K48" r:id="rId47" xr:uid="{D63EDBE2-BA4F-4AE1-AF14-7B86D2F69BDA}"/>
     <hyperlink ref="K47" r:id="rId48" xr:uid="{A1BDA74E-1F9A-4061-B250-267EFC06F2CC}"/>
     <hyperlink ref="K20" r:id="rId49" xr:uid="{E83A36DC-A6E2-4B10-8099-53E43FE4316B}"/>
+    <hyperlink ref="K49" r:id="rId50" xr:uid="{68C45329-3EDC-4BF4-8615-4876F956A3C1}"/>
+    <hyperlink ref="K50" r:id="rId51" xr:uid="{87383304-D3C0-4441-96E8-816A255794FC}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId50"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId52"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Dijital19 RNS gös. paralel hatası düzeltildi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137A4393-BA2E-4963-B7FF-9ED3A53613B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEB7953-96E9-483E-B24C-7A8837A8A44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,9 +225,6 @@
     <t>DP-D19-3X-NUV-CLI-S2B1-01</t>
   </si>
   <si>
-    <t>DP-D19-3X-RNS-CLI-P2B1-01</t>
-  </si>
-  <si>
     <t>DP-EKA-TF-ACM-COP-S2B1-01</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
     <t>https://github.com/btk42/DP-D19-3X-NUV-CLI-S2B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-D19-3X-RNS-CLI-P2B1-01</t>
-  </si>
-  <si>
     <t>2 Oklu 7Seg</t>
   </si>
   <si>
@@ -469,6 +463,12 @@
   </si>
   <si>
     <t>DP-D19-2X-NUV-CLI-P1B1-01</t>
+  </si>
+  <si>
+    <t>DP-D19-3X-RNS-CLI-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-D19-3X-RNS-CLI-S2B1-01</t>
   </si>
 </sst>
 </file>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K42" sqref="B42:K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -938,10 +938,10 @@
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -973,10 +973,10 @@
         <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -984,7 +984,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>20</v>
@@ -1008,10 +1008,10 @@
         <v>23</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1043,10 +1043,10 @@
         <v>23</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1078,10 +1078,10 @@
         <v>18</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1113,10 +1113,10 @@
         <v>18</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1148,10 +1148,10 @@
         <v>18</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1183,10 +1183,10 @@
         <v>18</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1218,10 +1218,10 @@
         <v>18</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1253,10 +1253,10 @@
         <v>18</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1288,10 +1288,10 @@
         <v>23</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1323,10 +1323,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1358,10 +1358,10 @@
         <v>23</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1393,10 +1393,10 @@
         <v>23</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1428,10 +1428,10 @@
         <v>23</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1439,10 +1439,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>44</v>
@@ -1463,10 +1463,10 @@
         <v>23</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L17" s="8"/>
     </row>
@@ -1475,10 +1475,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>44</v>
@@ -1499,10 +1499,10 @@
         <v>23</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L18" s="8"/>
     </row>
@@ -1511,7 +1511,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>32</v>
@@ -1535,10 +1535,10 @@
         <v>23</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1546,7 +1546,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>32</v>
@@ -1570,10 +1570,10 @@
         <v>23</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1581,7 +1581,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>41</v>
@@ -1605,10 +1605,10 @@
         <v>23</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1616,13 +1616,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>46</v>
@@ -1640,10 +1640,10 @@
         <v>23</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1675,10 +1675,10 @@
         <v>23</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1710,10 +1710,10 @@
         <v>23</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1745,10 +1745,10 @@
         <v>23</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1756,7 +1756,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>41</v>
@@ -1780,10 +1780,10 @@
         <v>23</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1815,10 +1815,10 @@
         <v>23</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1826,7 +1826,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>52</v>
@@ -1850,10 +1850,10 @@
         <v>23</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1861,7 +1861,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>52</v>
@@ -1885,10 +1885,10 @@
         <v>23</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1896,7 +1896,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>52</v>
@@ -1920,10 +1920,10 @@
         <v>23</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1931,7 +1931,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>52</v>
@@ -1955,10 +1955,10 @@
         <v>23</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1966,7 +1966,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>52</v>
@@ -1990,10 +1990,10 @@
         <v>23</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2001,7 +2001,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>52</v>
@@ -2025,10 +2025,10 @@
         <v>23</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2060,10 +2060,10 @@
         <v>18</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2095,10 +2095,10 @@
         <v>18</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2130,10 +2130,10 @@
         <v>23</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2165,10 +2165,10 @@
         <v>23</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2200,10 +2200,10 @@
         <v>23</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2211,7 +2211,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>32</v>
@@ -2235,10 +2235,10 @@
         <v>23</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2246,7 +2246,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>32</v>
@@ -2270,10 +2270,10 @@
         <v>23</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2305,10 +2305,10 @@
         <v>23</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2316,7 +2316,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>32</v>
@@ -2331,7 +2331,7 @@
         <v>54</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>22</v>
@@ -2340,10 +2340,10 @@
         <v>23</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2351,7 +2351,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>52</v>
@@ -2375,10 +2375,10 @@
         <v>23</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2386,10 +2386,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>53</v>
@@ -2398,7 +2398,7 @@
         <v>46</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>21</v>
@@ -2410,10 +2410,10 @@
         <v>23</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2421,10 +2421,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>13</v>
@@ -2445,10 +2445,10 @@
         <v>18</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2456,10 +2456,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>13</v>
@@ -2480,10 +2480,10 @@
         <v>18</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2491,13 +2491,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>48</v>
@@ -2515,10 +2515,10 @@
         <v>23</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2526,13 +2526,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>14</v>
@@ -2550,10 +2550,10 @@
         <v>23</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2561,13 +2561,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>48</v>
@@ -2585,10 +2585,10 @@
         <v>23</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2596,13 +2596,13 @@
         <v>50</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>48</v>
@@ -2620,10 +2620,10 @@
         <v>23</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LCD kablolu paralel bağlantı tipi düzeltildi.
</commit_message>
<xml_diff>
--- a/pages/gostergeler.xlsx
+++ b/pages/gostergeler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEB7953-96E9-483E-B24C-7A8837A8A44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40702CE-CE41-44FE-A546-332198DF5715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,9 +399,6 @@
     <t>DP-000-LC-NUV-LOP-P1B1-01</t>
   </si>
   <si>
-    <t>DP-000-LC-NUV-CLI-P1B1-01</t>
-  </si>
-  <si>
     <t>DP-000-TF-NUV-CLI-P2B1-01</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
     <t>https://github.com/btk42/DP-000-LC-NUV-LOP-P1B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/DP-000-LC-NUV-CLI-P1B1-01</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/DP-D19-3X-NUV-CLI-P1B1-01</t>
   </si>
   <si>
@@ -469,6 +463,12 @@
   </si>
   <si>
     <t>https://github.com/btk42/DP-D19-3X-RNS-CLI-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/DP-000-LC-NUV-CLI-P3B1-01</t>
+  </si>
+  <si>
+    <t>DP-000-LC-NUV-CLI-P3B1-01</t>
   </si>
 </sst>
 </file>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="B42:K42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1439,7 +1439,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>69</v>
@@ -1466,7 +1466,7 @@
         <v>68</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L17" s="8"/>
     </row>
@@ -1475,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>69</v>
@@ -1502,7 +1502,7 @@
         <v>68</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L18" s="8"/>
     </row>
@@ -1538,7 +1538,7 @@
         <v>68</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1573,7 +1573,7 @@
         <v>68</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1608,7 +1608,7 @@
         <v>68</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>68</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1888,7 +1888,7 @@
         <v>68</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1896,7 +1896,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>52</v>
@@ -1914,7 +1914,7 @@
         <v>16</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>23</v>
@@ -1923,7 +1923,7 @@
         <v>68</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2001,7 +2001,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>52</v>
@@ -2028,7 +2028,7 @@
         <v>68</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2211,7 +2211,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>32</v>
@@ -2238,7 +2238,7 @@
         <v>68</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2246,7 +2246,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>32</v>
@@ -2273,7 +2273,7 @@
         <v>68</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2316,7 +2316,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>32</v>
@@ -2343,7 +2343,7 @@
         <v>68</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2561,13 +2561,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>48</v>
@@ -2588,7 +2588,7 @@
         <v>68</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2596,13 +2596,13 @@
         <v>50</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>48</v>
@@ -2623,7 +2623,7 @@
         <v>68</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>